<commit_message>
R70 must be 0ohm, profiles corrected
</commit_message>
<xml_diff>
--- a/BOM/UniSolder52C_front_BOM.xlsx
+++ b/BOM/UniSolder52C_front_BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparky\Desktop\MyProjects\Electronics\UniSolder\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\UniSolder-5.2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1303B88B-5459-4276-ABCD-91E2CFD0EC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25068" windowHeight="13836"/>
+    <workbookView xWindow="7968" yWindow="3468" windowWidth="15552" windowHeight="10776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UniSolder52C_front" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="164">
   <si>
     <t>Designator</t>
   </si>
@@ -203,9 +204,6 @@
     <t>0805 Resistor</t>
   </si>
   <si>
-    <t>R23, R27, R28, R33, R44, R57, R70</t>
-  </si>
-  <si>
     <t>1.8k</t>
   </si>
   <si>
@@ -513,12 +511,21 @@
   </si>
   <si>
     <t>SOD123</t>
+  </si>
+  <si>
+    <t>R23, R27, R28, R33, R44, R57</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -861,13 +868,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1232,16 +1241,16 @@
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="4">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>56</v>
@@ -1255,16 +1264,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="4">
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>56</v>
@@ -1278,16 +1287,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>56</v>
@@ -1301,16 +1310,16 @@
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="4">
         <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>56</v>
@@ -1324,16 +1333,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>56</v>
@@ -1347,16 +1356,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>56</v>
@@ -1370,16 +1379,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="4">
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>56</v>
@@ -1393,16 +1402,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4">
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>56</v>
@@ -1416,16 +1425,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="4">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>56</v>
@@ -1439,16 +1448,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4">
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>56</v>
@@ -1462,16 +1471,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="4">
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>56</v>
@@ -1485,428 +1494,451 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B30" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E30" s="3" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B31" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B35" s="4">
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B38" s="4">
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B40" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B47" s="4">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="D48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>